<commit_message>
Second plot complete, but needs tweaking
</commit_message>
<xml_diff>
--- a/DW_Public_Genre_Order.xlsx
+++ b/DW_Public_Genre_Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selin\Desktop\UCD Data Analytics\UCDPA_Bayly_Selina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807E208B-4242-4409-B24E-0D3F43B5B479}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F59590C-04B9-4336-BF7B-CA40A560894B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,21 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
   <si>
     <t>The Colour of Magic</t>
   </si>
@@ -177,9 +168,6 @@
     <t>tLC</t>
   </si>
   <si>
-    <t>FE</t>
-  </si>
-  <si>
     <t>ToT</t>
   </si>
   <si>
@@ -198,9 +186,6 @@
     <t>MR</t>
   </si>
   <si>
-    <t>aJFoS</t>
-  </si>
-  <si>
     <t>GP</t>
   </si>
   <si>
@@ -454,6 +439,15 @@
   </si>
   <si>
     <t>The Amazing Maurice and His Educated Rodents</t>
+  </si>
+  <si>
+    <t>tFE</t>
+  </si>
+  <si>
+    <t>aHFoS</t>
+  </si>
+  <si>
+    <t>Display_Title</t>
   </si>
 </sst>
 </file>
@@ -782,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G7" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,32 +791,36 @@
     <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -833,19 +831,23 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G2" s="3">
         <v>1983</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="str">
+        <f>A2&amp;". "&amp;B2</f>
+        <v>1. The Colour of Magic</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -856,19 +858,23 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G3" s="3">
         <v>1986</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H42" si="0">A3&amp;". "&amp;B3</f>
+        <v>2. The Light Fantastic</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -879,19 +885,23 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G4" s="3">
         <v>1987</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>3. Equal Rites</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -899,22 +909,26 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G5" s="3">
         <v>1987</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>4. Mort</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -922,22 +936,26 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
-        <v>64</v>
-      </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G6" s="3">
         <v>1988</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>5. Sourcery</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -948,19 +966,23 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G7" s="3">
         <v>1988</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>6. Wyrd Sisters</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -971,19 +993,23 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G8" s="3">
         <v>1989</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>7. Pyramids</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -994,42 +1020,50 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G9" s="3">
         <v>1989</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>8. Guards! Guards!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G10" s="3">
         <v>1990</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>9. Eric</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1040,19 +1074,23 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G11" s="3">
         <v>1990</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>10. Moving Pictures</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1063,19 +1101,23 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G12" s="3">
         <v>1991</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>11. Reaper Man</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1086,19 +1128,23 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G13" s="3">
         <v>1991</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>12. Witches Abroad</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1109,19 +1155,23 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G14" s="3">
         <v>1992</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>13. Small Gods</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1132,42 +1182,50 @@
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G15" s="3">
         <v>1992</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>14. Lords and Ladies</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
         <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G16" s="3">
         <v>1993</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>15. Men at Arms</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1178,19 +1236,23 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G17" s="3">
         <v>1994</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>16. Soul Music</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1201,19 +1263,23 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G18" s="3">
         <v>1994</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>17. Interesting Times</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1224,19 +1290,23 @@
         <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G19" s="3">
         <v>1995</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>18. Maskerade</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1247,19 +1317,23 @@
         <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G20" s="3">
         <v>1996</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>19. Feet of Clay</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1270,19 +1344,23 @@
         <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G21" s="3">
         <v>1996</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>20. Hogfather</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1293,19 +1371,23 @@
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G22" s="3">
         <v>1997</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>21. Jingo</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1316,19 +1398,23 @@
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G23" s="3">
         <v>1998</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>22. The Last Continent</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1339,19 +1425,23 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G24" s="3">
         <v>1998</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>23. Carpe Jugulum</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1359,68 +1449,80 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G25" s="3">
         <v>1999</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>24. The Fifth Elephant</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G26" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>25. The Truth</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G27" s="3">
         <v>2001</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>26. Thief of Time</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1428,341 +1530,401 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G28" s="3">
         <v>2001</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>27. The Last Hero</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G29" s="3">
         <v>2001</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>28. The Amazing Maurice and His Educated Rodents</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G30" s="3">
         <v>2002</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>29. Night Watch</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G31" s="3">
         <v>2003</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>30. The Wee Free Men</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G32" s="3">
         <v>2003</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>31. Monstrous Regiment</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G33" s="3">
         <v>2004</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>32. A Hat Full of Sky</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G34" s="3">
         <v>2004</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>33. Going Postal</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G35" s="3">
         <v>2005</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>34. Thud!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G36" s="3">
         <v>2006</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>35. Wintersmith</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G37" s="3">
         <v>2007</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>36. Making Money</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G38" s="3">
         <v>2009</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>37. Unseen Academicals</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G39" s="3">
         <v>2010</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>38. I Shall Wear Midnight</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G40" s="3">
         <v>2011</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>39. Snuff</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G41" s="3">
         <v>2013</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>40. Raising Steam</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G42" s="3">
         <v>2015</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>41. The Shepherd's Crown</v>
       </c>
     </row>
   </sheetData>

</xml_diff>